<commit_message>
đã test các thay đổi mới
</commit_message>
<xml_diff>
--- a/vdm_lk2_machine/database/form_khsx_cdth.xlsx
+++ b/vdm_lk2_machine/database/form_khsx_cdth.xlsx
@@ -552,149 +552,124 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40000</v>
+        <v>35748</v>
       </c>
       <c r="D3" t="n">
-        <v>38160</v>
+        <v>8504</v>
       </c>
       <c r="E3" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>38160</v>
+        <v>16284</v>
       </c>
       <c r="G3" t="n">
-        <v>38160</v>
+        <v>1148</v>
       </c>
       <c r="H3" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>53.0061349693252</v>
+        <v>49.6551724137931</v>
       </c>
       <c r="J3" t="n">
-        <v>53.0061349693252</v>
+        <v>49.6551724137931</v>
       </c>
       <c r="K3" t="n">
-        <v>53.0061349693252</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>53.0061349693252</v>
+        <v>22.61780104712042</v>
       </c>
       <c r="M3" t="n">
-        <v>53.0061349693252</v>
+        <v>22.61780104712042</v>
       </c>
       <c r="N3" t="n">
-        <v>53.0061349693252</v>
+        <v>0</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>04148XA</t>
+          <t>04162XA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>04148XA</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>04148XA</t>
-        </is>
-      </c>
+          <t>04162XA</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>04148XA</t>
+          <t>04143XA</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>04148XA</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>04148XA</t>
-        </is>
-      </c>
+          <t>04143XA</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>J01</t>
-        </is>
-      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>38160</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>30240</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>53.0061349693252</v>
+        <v>49.6551724137931</v>
       </c>
       <c r="J4" t="n">
-        <v>53.0061349693252</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>53.0061349693252</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>53.0061349693252</v>
+        <v>22.61780104712042</v>
       </c>
       <c r="M4" t="n">
-        <v>53.0061349693252</v>
+        <v>22.61780104712042</v>
       </c>
       <c r="N4" t="n">
-        <v>53.0061349693252</v>
+        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>04148XA</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>04148XA</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>04148XA</t>
-        </is>
-      </c>
+          <t>04162XA</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
-          <t>04148XA</t>
+          <t>04143XA</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>04148XA</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>04148XA</t>
-        </is>
-      </c>
+          <t>04143XA</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -714,7 +689,7 @@
         <v>293988</v>
       </c>
       <c r="E5" t="n">
-        <v>236072</v>
+        <v>142084</v>
       </c>
       <c r="F5" t="n">
         <v>293988</v>
@@ -726,16 +701,16 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="J5" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="K5" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="L5" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -763,6 +738,8 @@
           <t>15E09XB</t>
         </is>
       </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -776,7 +753,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>293988</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>293988</v>
@@ -785,7 +762,7 @@
         <v>293988</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>293988</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -794,16 +771,16 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>408.317580340265</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="K6" t="n">
-        <v>408.317580340265</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>408.3175803402647</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -811,21 +788,24 @@
       <c r="N6" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
         <is>
           <t>15E09XB</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>15E09XB</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>15E09XB</t>
         </is>
       </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -839,7 +819,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>12084</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -857,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>15.0313152400835</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -874,11 +854,12 @@
       <c r="N7" t="n">
         <v>0</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>49551XA</t>
-        </is>
-      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -892,7 +873,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7916</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -910,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>15.0313152400835</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -927,11 +908,12 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>49551XA</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -945,69 +927,57 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4903</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>4903</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>4903</v>
       </c>
       <c r="F9" t="n">
-        <v>582</v>
+        <v>4903</v>
       </c>
       <c r="G9" t="n">
-        <v>4903</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>4903</v>
       </c>
       <c r="I9" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>7.5</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>7.5</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="M9" t="n">
-        <v>8.05068952664927</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>8.05068952664927</v>
-      </c>
-      <c r="O9" t="inlineStr">
+        <v>7.500000000000001</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>32BQPXB</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>32BQPXB</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
         <is>
           <t>32BQPXB</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>32BQPXB</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>32BQNXB</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>32BQNXB</t>
         </is>
       </c>
     </row>
@@ -1023,7 +993,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4903</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>4903</v>
@@ -1032,60 +1002,56 @@
         <v>4903</v>
       </c>
       <c r="F10" t="n">
-        <v>388</v>
+        <v>4903</v>
       </c>
       <c r="G10" t="n">
         <v>4903</v>
       </c>
       <c r="H10" t="n">
-        <v>4903</v>
+        <v>679</v>
       </c>
       <c r="I10" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>7.5</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="K10" t="n">
-        <v>7.5</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="L10" t="n">
-        <v>8.05068952664927</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="M10" t="n">
-        <v>8.05068952664927</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="N10" t="n">
-        <v>8.05068952664927</v>
-      </c>
-      <c r="O10" t="inlineStr">
+        <v>7.500000000000001</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
         <is>
           <t>32BQPXB</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>32BQPXB</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>32BQPXB</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>32BQNXB</t>
-        </is>
-      </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>32BQNXB</t>
+          <t>32BQPXB</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>32BQNXB</t>
+          <t>32BQPXB</t>
         </is>
       </c>
     </row>
@@ -1113,25 +1079,25 @@
         <v>42404</v>
       </c>
       <c r="G11" t="n">
-        <v>5768</v>
+        <v>10768</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="J11" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="K11" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="L11" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="M11" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -1161,6 +1127,7 @@
           <t>32BKVXB</t>
         </is>
       </c>
+      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1174,7 +1141,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>42404</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>42404</v>
@@ -1189,44 +1156,46 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="I12" t="n">
-        <v>57.9865771812081</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="K12" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="L12" t="n">
-        <v>57.9865771812081</v>
+        <v>57.98657718120805</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="inlineStr">
+        <v>26.66666666666667</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
         <is>
           <t>32BKVXB</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>32BKVXB</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>32BKVXB</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>32BKVXB</t>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>32BRZXB</t>
         </is>
       </c>
     </row>
@@ -1245,37 +1214,43 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="E13" t="n">
-        <v>19550</v>
+        <v>30000</v>
       </c>
       <c r="F13" t="n">
-        <v>19550</v>
+        <v>53856</v>
       </c>
       <c r="G13" t="n">
-        <v>19550</v>
+        <v>53856</v>
       </c>
       <c r="H13" t="n">
-        <v>19550</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>27.15273412947831</v>
       </c>
       <c r="K13" t="n">
-        <v>27.1527341294783</v>
+        <v>27.15273412947831</v>
       </c>
       <c r="L13" t="n">
-        <v>27.1527341294783</v>
+        <v>74.8051948051948</v>
       </c>
       <c r="M13" t="n">
-        <v>27.1527341294783</v>
+        <v>74.8051948051948</v>
       </c>
       <c r="N13" t="n">
-        <v>27.1527341294783</v>
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>32BRHXA</t>
+        </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1284,19 +1259,15 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
+          <t>43D50XA</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>32BRHXA</t>
-        </is>
-      </c>
+          <t>43D50XA</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1313,38 +1284,39 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>18600</v>
+        <v>30000</v>
       </c>
       <c r="E14" t="n">
-        <v>19550</v>
+        <v>53720</v>
       </c>
       <c r="F14" t="n">
-        <v>19550</v>
+        <v>53856</v>
       </c>
       <c r="G14" t="n">
-        <v>19550</v>
+        <v>53856</v>
       </c>
       <c r="H14" t="n">
-        <v>19550</v>
+        <v>53856</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>27.1527341294783</v>
+        <v>27.15273412947831</v>
       </c>
       <c r="K14" t="n">
-        <v>27.1527341294783</v>
+        <v>74.8051948051948</v>
       </c>
       <c r="L14" t="n">
-        <v>27.1527341294783</v>
+        <v>74.8051948051948</v>
       </c>
       <c r="M14" t="n">
-        <v>27.1527341294783</v>
+        <v>74.8051948051948</v>
       </c>
       <c r="N14" t="n">
-        <v>27.1527341294783</v>
-      </c>
+        <v>74.8051948051948</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
           <t>32BRHXA</t>
@@ -1352,22 +1324,22 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
+          <t>43D50XA</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
+          <t>43D50XA</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
+          <t>43D50XA</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>32BRHXA</t>
+          <t>43D50XA</t>
         </is>
       </c>
     </row>
@@ -1386,13 +1358,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>65340</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>65340</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>65340</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -1404,13 +1376,13 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
@@ -1418,6 +1390,24 @@
       <c r="N15" t="n">
         <v>0</v>
       </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1434,13 +1424,13 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>65340</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>65340</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>53300</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -1452,13 +1442,13 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>90.75630252100841</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -1466,6 +1456,24 @@
       <c r="N16" t="n">
         <v>0</v>
       </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>32BSGXA</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1479,10 +1487,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>67034</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>45000</v>
+        <v>71256</v>
       </c>
       <c r="E17" t="n">
         <v>71256</v>
@@ -1494,54 +1502,50 @@
         <v>71256</v>
       </c>
       <c r="H17" t="n">
-        <v>71256</v>
+        <v>67034</v>
       </c>
       <c r="I17" t="n">
-        <v>93.10344827586211</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>95.2590959206174</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="K17" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="L17" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="M17" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="N17" t="n">
-        <v>98.9690721649485</v>
-      </c>
-      <c r="O17" t="inlineStr">
+        <v>93.10344827586206</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
         <is>
           <t>32C99XA</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>32BLBXA</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>31788AB</t>
         </is>
       </c>
     </row>
@@ -1557,10 +1561,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>22966</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>71208</v>
+        <v>71256</v>
       </c>
       <c r="E18" t="n">
         <v>71256</v>
@@ -1569,52 +1573,53 @@
         <v>71256</v>
       </c>
       <c r="G18" t="n">
-        <v>71256</v>
+        <v>39952</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>27966</v>
       </c>
       <c r="I18" t="n">
-        <v>93.10344827586211</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="K18" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="L18" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="M18" t="n">
-        <v>98.9690721649485</v>
+        <v>98.96907216494846</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="inlineStr">
+        <v>93.10344827586206</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>31788AB</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
         <is>
           <t>32C99XA</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>31788AB</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>31788AB</t>
         </is>
       </c>
     </row>
@@ -1630,7 +1635,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>35615</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>35615</v>
@@ -1648,28 +1653,24 @@
         <v>35615</v>
       </c>
       <c r="I19" t="n">
-        <v>49.4656488549618</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="K19" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="L19" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="M19" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="N19" t="n">
-        <v>49.4656488549618</v>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>32BQ7XA</t>
-        </is>
-      </c>
+        <v>49.46564885496183</v>
+      </c>
+      <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
           <t>32BQ7XA</t>
@@ -1708,7 +1709,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34625</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>35615</v>
@@ -1726,28 +1727,24 @@
         <v>35615</v>
       </c>
       <c r="I20" t="n">
-        <v>49.4656488549618</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="K20" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="L20" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="M20" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="N20" t="n">
-        <v>49.4656488549618</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>32BQ7XA</t>
-        </is>
-      </c>
+        <v>49.46564885496183</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
           <t>32BQ7XA</t>
@@ -1786,16 +1783,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34560</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>34560</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>34560</v>
+        <v>14920</v>
       </c>
       <c r="F21" t="n">
-        <v>34560</v>
+        <v>35615</v>
       </c>
       <c r="G21" t="n">
         <v>35615</v>
@@ -1804,41 +1801,33 @@
         <v>35615</v>
       </c>
       <c r="I21" t="n">
-        <v>55.6701030927835</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>55.6701030927835</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>55.6701030927835</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="L21" t="n">
-        <v>55.6701030927835</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="M21" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="N21" t="n">
-        <v>49.4656488549618</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>32BPVXA</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>32BPVXA</t>
-        </is>
-      </c>
+        <v>49.46564885496183</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>32BPVXA</t>
+          <t>32BQ7XA</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>32BPVXA</t>
+          <t>32BQ7XA</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -1864,16 +1853,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>30000</v>
+        <v>35600</v>
       </c>
       <c r="D22" t="n">
-        <v>34560</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>34560</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>35150</v>
+        <v>35615</v>
       </c>
       <c r="G22" t="n">
         <v>35615</v>
@@ -1882,38 +1871,30 @@
         <v>35615</v>
       </c>
       <c r="I22" t="n">
-        <v>55.6701030927835</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="J22" t="n">
-        <v>55.6701030927835</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>55.6701030927835</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="M22" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="N22" t="n">
-        <v>49.4656488549618</v>
+        <v>49.46564885496183</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>32BPVXA</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>32BPVXA</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>32BPVXA</t>
-        </is>
-      </c>
+          <t>32BQ7XA</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
         <is>
           <t>32BQ7XA</t>
@@ -1942,7 +1923,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>62832</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>62832</v>
@@ -1957,31 +1938,27 @@
         <v>62832</v>
       </c>
       <c r="H23" t="n">
-        <v>62832</v>
+        <v>23512</v>
       </c>
       <c r="I23" t="n">
-        <v>87.27272727272729</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="K23" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="L23" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="M23" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="N23" t="n">
-        <v>87.27272727272729</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>14332AA</t>
-        </is>
-      </c>
+        <v>87.27272727272727</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
           <t>14332AA</t>
@@ -2023,7 +2000,7 @@
         <v>62832</v>
       </c>
       <c r="D24" t="n">
-        <v>62832</v>
+        <v>61000</v>
       </c>
       <c r="E24" t="n">
         <v>62832</v>
@@ -2035,25 +2012,25 @@
         <v>62832</v>
       </c>
       <c r="H24" t="n">
-        <v>62832</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="J24" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="K24" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="L24" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="M24" t="n">
-        <v>87.27272727272729</v>
+        <v>87.27272727272727</v>
       </c>
       <c r="N24" t="n">
-        <v>87.27272727272729</v>
+        <v>0</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2080,11 +2057,7 @@
           <t>14332AA</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>14332AA</t>
-        </is>
-      </c>
+      <c r="T24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2098,56 +2071,45 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>46016</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>16548</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>16548</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>16548</v>
       </c>
       <c r="H25" t="n">
-        <v>712</v>
+        <v>8904</v>
       </c>
       <c r="I25" t="n">
-        <v>87.27272727272729</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>22.9787234042553</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>22.9787234042553</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>22.9787234042553</v>
+        <v>22.97872340425532</v>
       </c>
       <c r="N25" t="n">
-        <v>22.9787234042553</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>14332AA</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>43G88XA</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>43G88XA</t>
-        </is>
-      </c>
+        <v>22.97872340425532</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
           <t>43G88XA</t>
@@ -2177,10 +2139,10 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>16548</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>16548</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
         <v>16548</v>
@@ -2195,32 +2157,27 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>22.9787234042553</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>22.9787234042553</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>22.9787234042553</v>
+        <v>22.97872340425532</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
         <is>
           <t>43G88XA</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>43G88XA</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>43G88XA</t>
-        </is>
-      </c>
+      <c r="T26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2234,71 +2191,55 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>74000</v>
       </c>
       <c r="E27" t="n">
-        <v>74000</v>
+        <v>24000</v>
       </c>
       <c r="F27" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>102.857142857143</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="K27" t="n">
-        <v>102.857142857143</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="L27" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>102.857142857143</v>
-      </c>
-      <c r="O27" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
         <is>
           <t>31873AA</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="Q27" t="inlineStr">
         <is>
           <t>31873AA</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2318,34 +2259,34 @@
         <v>74000</v>
       </c>
       <c r="E28" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>74000</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>102.857142857143</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="J28" t="n">
-        <v>102.857142857143</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="K28" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>102.857142857143</v>
+        <v>0</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2357,26 +2298,10 @@
           <t>31873AA</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>31873AA</t>
-        </is>
-      </c>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2390,10 +2315,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>62899</v>
+        <v>52896</v>
       </c>
       <c r="D29" t="n">
-        <v>40000</v>
+        <v>52896</v>
       </c>
       <c r="E29" t="n">
         <v>69744</v>
@@ -2402,37 +2327,37 @@
         <v>69744</v>
       </c>
       <c r="G29" t="n">
-        <v>34872</v>
+        <v>69744</v>
       </c>
       <c r="H29" t="n">
-        <v>52896</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>87.360970677452</v>
+        <v>73.46938775510202</v>
       </c>
       <c r="J29" t="n">
-        <v>86.4864864864865</v>
+        <v>73.46938775510202</v>
       </c>
       <c r="K29" t="n">
-        <v>108.40652446675</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="L29" t="n">
-        <v>108.40652446675</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="M29" t="n">
-        <v>108.40652446675</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="N29" t="n">
-        <v>73.46938775510201</v>
+        <v>0</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>32Y28XA</t>
+          <t>43D28XA</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>32R29XA</t>
+          <t>43D28XA</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -2450,11 +2375,7 @@
           <t>32R28XA</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>43D28XA</t>
-        </is>
-      </c>
+      <c r="T29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2468,10 +2389,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>7101</v>
+        <v>52896</v>
       </c>
       <c r="D30" t="n">
-        <v>16152</v>
+        <v>22912</v>
       </c>
       <c r="E30" t="n">
         <v>69744</v>
@@ -2480,59 +2401,55 @@
         <v>69744</v>
       </c>
       <c r="G30" t="n">
-        <v>52896</v>
+        <v>1280</v>
       </c>
       <c r="H30" t="n">
-        <v>18208</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>87.360970677452</v>
+        <v>73.46938775510202</v>
       </c>
       <c r="J30" t="n">
-        <v>108.40652446675</v>
+        <v>73.46938775510202</v>
       </c>
       <c r="K30" t="n">
-        <v>108.40652446675</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="L30" t="n">
-        <v>108.40652446675</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="M30" t="n">
-        <v>73.46938775510201</v>
+        <v>108.4065244667503</v>
       </c>
       <c r="N30" t="n">
-        <v>73.46938775510201</v>
+        <v>0</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>32Y28XA</t>
+          <t>43D28XA</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
+          <t>43D28XA</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
           <t>32R28XA</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="R30" t="inlineStr">
         <is>
           <t>32R28XA</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr">
+      <c r="S30" t="inlineStr">
         <is>
           <t>32R28XA</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>43D28XA</t>
-        </is>
-      </c>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>43D28XA</t>
-        </is>
-      </c>
+      <c r="T30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2546,13 +2463,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>65340</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>65340</v>
+        <v>50000</v>
       </c>
       <c r="E31" t="n">
-        <v>65688</v>
+        <v>60000</v>
       </c>
       <c r="F31" t="n">
         <v>65688</v>
@@ -2561,54 +2478,50 @@
         <v>65688</v>
       </c>
       <c r="H31" t="n">
-        <v>65340</v>
+        <v>64000</v>
       </c>
       <c r="I31" t="n">
-        <v>90.75630252100839</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>90.75630252100839</v>
+        <v>105.3658536585366</v>
       </c>
       <c r="K31" t="n">
-        <v>91.2354804646251</v>
+        <v>105.3658536585366</v>
       </c>
       <c r="L31" t="n">
-        <v>91.2354804646251</v>
+        <v>91.23548046462514</v>
       </c>
       <c r="M31" t="n">
-        <v>91.2354804646251</v>
+        <v>91.23548046462514</v>
       </c>
       <c r="N31" t="n">
-        <v>90.75630252100839</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>32BSGXA</t>
-        </is>
-      </c>
+        <v>91.23548046462514</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>32BSGXA</t>
+          <t>31757AA</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
+          <t>31757AA</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
           <t>32R37XA</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
+      <c r="S31" t="inlineStr">
         <is>
           <t>32R37XA</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="T31" t="inlineStr">
         <is>
           <t>32R37XA</t>
-        </is>
-      </c>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>32BSGXA</t>
         </is>
       </c>
     </row>
@@ -2624,69 +2537,65 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>65340</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>65688</v>
+        <v>60000</v>
       </c>
       <c r="E32" t="n">
-        <v>65688</v>
+        <v>60000</v>
       </c>
       <c r="F32" t="n">
         <v>65688</v>
       </c>
       <c r="G32" t="n">
-        <v>49172</v>
+        <v>65688</v>
       </c>
       <c r="H32" t="n">
-        <v>65340</v>
+        <v>23248</v>
       </c>
       <c r="I32" t="n">
-        <v>90.75630252100839</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>91.2354804646251</v>
+        <v>105.3658536585366</v>
       </c>
       <c r="K32" t="n">
-        <v>91.2354804646251</v>
+        <v>105.3658536585366</v>
       </c>
       <c r="L32" t="n">
-        <v>91.2354804646251</v>
+        <v>91.23548046462514</v>
       </c>
       <c r="M32" t="n">
-        <v>91.2354804646251</v>
+        <v>91.23548046462514</v>
       </c>
       <c r="N32" t="n">
-        <v>90.75630252100839</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>32BSGXA</t>
-        </is>
-      </c>
+        <v>91.23548046462514</v>
+      </c>
+      <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
+          <t>31757AA</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>31757AA</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
           <t>32R37XA</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
+      <c r="S32" t="inlineStr">
         <is>
           <t>32R37XA</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>32R37XA</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>32R37XA</t>
-        </is>
-      </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>32BSGXA</t>
         </is>
       </c>
     </row>
@@ -2702,71 +2611,63 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>15000</v>
+        <v>23916</v>
       </c>
       <c r="D33" t="n">
-        <v>6752</v>
+        <v>17168</v>
       </c>
       <c r="E33" t="n">
-        <v>41472</v>
+        <v>21012</v>
       </c>
       <c r="F33" t="n">
-        <v>41472</v>
+        <v>21012</v>
       </c>
       <c r="G33" t="n">
-        <v>41472</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>41472</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>32.8267477203647</v>
+        <v>33.48837209302327</v>
       </c>
       <c r="J33" t="n">
-        <v>30.6382978723404</v>
+        <v>33.48837209302327</v>
       </c>
       <c r="K33" t="n">
-        <v>30.6382978723404</v>
+        <v>29.18918918918918</v>
       </c>
       <c r="L33" t="n">
-        <v>30.6382978723404</v>
+        <v>29.18918918918918</v>
       </c>
       <c r="M33" t="n">
-        <v>30.6382978723404</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>30.6382978723404</v>
+        <v>0</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>32BS6XA</t>
+          <t>32BTJXB</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>32BQ9XC</t>
+          <t>32BTJXB</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>32BQ9XC</t>
+          <t>32BTHXA</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
+          <t>32BTHXA</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2780,71 +2681,59 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>15000</v>
+        <v>23916</v>
       </c>
       <c r="D34" t="n">
-        <v>41472</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>41472</v>
+        <v>21012</v>
       </c>
       <c r="F34" t="n">
-        <v>41472</v>
+        <v>1964</v>
       </c>
       <c r="G34" t="n">
-        <v>41472</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>41472</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>32.8267477203647</v>
+        <v>33.48837209302327</v>
       </c>
       <c r="J34" t="n">
-        <v>30.6382978723404</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>30.6382978723404</v>
+        <v>29.18918918918918</v>
       </c>
       <c r="L34" t="n">
-        <v>30.6382978723404</v>
+        <v>29.18918918918918</v>
       </c>
       <c r="M34" t="n">
-        <v>30.6382978723404</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>30.6382978723404</v>
+        <v>0</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>32BS6XA</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
+          <t>32BTJXB</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>32BQ9XC</t>
+          <t>32BTHXA</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>32BQ9XC</t>
-        </is>
-      </c>
+          <t>32BTHXA</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2858,16 +2747,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>42024</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>34560</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>34560</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>34560</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -2876,16 +2765,16 @@
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>58.3783783783784</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>55.6701030927835</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>55.6701030927835</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>55.6701030927835</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
@@ -2893,11 +2782,24 @@
       <c r="N35" t="n">
         <v>0</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>32BL3XA</t>
-        </is>
-      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>32BPVXA</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>32BPVXA</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>32BPVXA</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2911,13 +2813,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7976</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>34560</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>34560</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -2929,13 +2831,13 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>58.3783783783784</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>55.6701030927835</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>55.6701030927835</v>
       </c>
       <c r="L36" t="n">
         <v>0</v>
@@ -2946,11 +2848,20 @@
       <c r="N36" t="n">
         <v>0</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>32BL3XA</t>
-        </is>
-      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>32BPVXA</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>32BPVXA</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2964,7 +2875,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>79044</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>79044</v>
@@ -2982,28 +2893,24 @@
         <v>79044</v>
       </c>
       <c r="I37" t="n">
-        <v>110.063694267516</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="K37" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="L37" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="M37" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="N37" t="n">
-        <v>110.063694267516</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>32BS3XA</t>
-        </is>
-      </c>
+        <v>110.0636942675159</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
           <t>32BS3XA</t>
@@ -3042,7 +2949,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>79044</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>79044</v>
@@ -3051,7 +2958,7 @@
         <v>79044</v>
       </c>
       <c r="F38" t="n">
-        <v>77068</v>
+        <v>78261</v>
       </c>
       <c r="G38" t="n">
         <v>79044</v>
@@ -3060,28 +2967,24 @@
         <v>79044</v>
       </c>
       <c r="I38" t="n">
-        <v>110.063694267516</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="K38" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="L38" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="M38" t="n">
-        <v>110.063694267516</v>
+        <v>110.0636942675159</v>
       </c>
       <c r="N38" t="n">
-        <v>110.063694267516</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>32BS3XA</t>
-        </is>
-      </c>
+        <v>110.0636942675159</v>
+      </c>
+      <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
           <t>32BS3XA</t>
@@ -3120,64 +3023,60 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>75864</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="E39" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="F39" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="G39" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="H39" t="n">
-        <v>42000</v>
+        <v>74000</v>
       </c>
       <c r="I39" t="n">
-        <v>105.365853658537</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="K39" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="L39" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="M39" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="N39" t="n">
-        <v>102.857142857143</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>31757AA</t>
-        </is>
-      </c>
+        <v>102.8571428571429</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
@@ -3198,64 +3097,60 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>75864</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="E40" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="F40" t="n">
-        <v>75864</v>
+        <v>74000</v>
       </c>
       <c r="G40" t="n">
-        <v>17224</v>
+        <v>64000</v>
       </c>
       <c r="H40" t="n">
         <v>74000</v>
       </c>
       <c r="I40" t="n">
-        <v>105.365853658537</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="K40" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="L40" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="M40" t="n">
-        <v>105.365853658537</v>
+        <v>102.8571428571429</v>
       </c>
       <c r="N40" t="n">
-        <v>102.857142857143</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>31757AA</t>
-        </is>
-      </c>
+        <v>102.8571428571429</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>31757AA</t>
+          <t>31873AA</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -3276,7 +3171,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>278124</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
         <v>278124</v>
@@ -3285,50 +3180,51 @@
         <v>278124</v>
       </c>
       <c r="F41" t="n">
-        <v>131256</v>
+        <v>81256</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>9816</v>
       </c>
       <c r="H41" t="n">
         <v>12156</v>
       </c>
       <c r="I41" t="n">
-        <v>386.28912071535</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>386.28912071535</v>
+        <v>386.2891207153502</v>
       </c>
       <c r="K41" t="n">
-        <v>386.28912071535</v>
+        <v>386.2891207153502</v>
       </c>
       <c r="L41" t="n">
-        <v>386.28912071535</v>
+        <v>386.2891207153502</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>16.875</v>
       </c>
       <c r="N41" t="n">
         <v>16.875</v>
       </c>
-      <c r="O41" t="inlineStr">
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
         <is>
           <t>15B24XB</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr">
+      <c r="Q41" t="inlineStr">
         <is>
           <t>15B24XB</t>
         </is>
       </c>
-      <c r="Q41" t="inlineStr">
+      <c r="R41" t="inlineStr">
         <is>
           <t>15B24XB</t>
         </is>
       </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>15B24XB</t>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>04171XA</t>
         </is>
       </c>
       <c r="T41" t="inlineStr">
@@ -3349,7 +3245,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>278124</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
         <v>278124</v>
@@ -3364,16 +3260,16 @@
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>11972</v>
+        <v>12156</v>
       </c>
       <c r="I42" t="n">
-        <v>386.28912071535</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>386.28912071535</v>
+        <v>386.2891207153502</v>
       </c>
       <c r="K42" t="n">
-        <v>386.28912071535</v>
+        <v>386.2891207153502</v>
       </c>
       <c r="L42" t="n">
         <v>0</v>
@@ -3384,21 +3280,19 @@
       <c r="N42" t="n">
         <v>16.875</v>
       </c>
-      <c r="O42" t="inlineStr">
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
         <is>
           <t>15B24XB</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
+      <c r="Q42" t="inlineStr">
         <is>
           <t>15B24XB</t>
         </is>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>15B24XB</t>
-        </is>
-      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr">
         <is>
           <t>04171XA</t>
@@ -3417,7 +3311,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>12156</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>12156</v>
@@ -3435,7 +3329,7 @@
         <v>12156</v>
       </c>
       <c r="I43" t="n">
-        <v>16.875</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
         <v>16.875</v>
@@ -3452,11 +3346,7 @@
       <c r="N43" t="n">
         <v>16.875</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>04171XA</t>
-        </is>
-      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
           <t>04171XA</t>
@@ -3495,7 +3385,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12156</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>12156</v>
@@ -3513,7 +3403,7 @@
         <v>12156</v>
       </c>
       <c r="I44" t="n">
-        <v>16.875</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
         <v>16.875</v>
@@ -3530,11 +3420,7 @@
       <c r="N44" t="n">
         <v>16.875</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>04171XA</t>
-        </is>
-      </c>
+      <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
           <t>04171XA</t>
@@ -3573,13 +3459,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4690</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>5531</v>
       </c>
       <c r="E45" t="n">
-        <v>5531</v>
+        <v>5000</v>
       </c>
       <c r="F45" t="n">
         <v>5531</v>
@@ -3588,56 +3474,48 @@
         <v>5531</v>
       </c>
       <c r="H45" t="n">
-        <v>5531</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>7.68136557610242</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="K45" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="L45" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="M45" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="N45" t="n">
-        <v>7.68136557610242</v>
-      </c>
-      <c r="O45" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="Q45" t="inlineStr">
+      <c r="R45" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="R45" t="inlineStr">
+      <c r="S45" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>22D70XA</t>
-        </is>
-      </c>
-      <c r="T45" t="inlineStr">
-        <is>
-          <t>22D70XA</t>
-        </is>
-      </c>
+      <c r="T45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3651,52 +3529,53 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5531</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>5531</v>
       </c>
       <c r="E46" t="n">
-        <v>5531</v>
+        <v>5000</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>2345</v>
       </c>
       <c r="G46" t="n">
         <v>5531</v>
       </c>
       <c r="H46" t="n">
-        <v>5531</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>7.68136557610242</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="K46" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="M46" t="n">
-        <v>7.68136557610242</v>
+        <v>7.681365576102417</v>
       </c>
       <c r="N46" t="n">
-        <v>7.68136557610242</v>
-      </c>
-      <c r="O46" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
+      <c r="Q46" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="Q46" t="inlineStr">
+      <c r="R46" t="inlineStr">
         <is>
           <t>22D70XA</t>
         </is>
@@ -3706,11 +3585,7 @@
           <t>22D70XA</t>
         </is>
       </c>
-      <c r="T46" t="inlineStr">
-        <is>
-          <t>22D70XA</t>
-        </is>
-      </c>
+      <c r="T46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3759,6 +3634,12 @@
       <c r="N47" t="n">
         <v>0</v>
       </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3807,6 +3688,12 @@
       <c r="N48" t="n">
         <v>0</v>
       </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3835,25 +3722,25 @@
         <v>7353</v>
       </c>
       <c r="H49" t="n">
-        <v>6470</v>
+        <v>7353</v>
       </c>
       <c r="I49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="J49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="K49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="L49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="M49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="N49" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -3898,7 +3785,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>7353</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
         <v>7353</v>
@@ -3913,54 +3800,50 @@
         <v>7353</v>
       </c>
       <c r="H50" t="n">
-        <v>20000</v>
+        <v>4117</v>
       </c>
       <c r="I50" t="n">
-        <v>10.2127659574468</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="K50" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="L50" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="M50" t="n">
-        <v>10.2127659574468</v>
+        <v>10.21276595744681</v>
       </c>
       <c r="N50" t="n">
-        <v>26.6666666666667</v>
-      </c>
-      <c r="O50" t="inlineStr">
+        <v>10.21276595744681</v>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
         <is>
           <t>31865AA</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
+      <c r="Q50" t="inlineStr">
         <is>
           <t>31865AA</t>
         </is>
       </c>
-      <c r="Q50" t="inlineStr">
+      <c r="R50" t="inlineStr">
         <is>
           <t>31865AA</t>
         </is>
       </c>
-      <c r="R50" t="inlineStr">
+      <c r="S50" t="inlineStr">
         <is>
           <t>31865AA</t>
         </is>
       </c>
-      <c r="S50" t="inlineStr">
+      <c r="T50" t="inlineStr">
         <is>
           <t>31865AA</t>
-        </is>
-      </c>
-      <c r="T50" t="inlineStr">
-        <is>
-          <t>32BRZXB</t>
         </is>
       </c>
     </row>

</xml_diff>